<commit_message>
Cost moyeu avant et roue
</commit_message>
<xml_diff>
--- a/WT - Wheels, Wheel Bearing & Tires/Cost/WT A0100 (Wheel Assembly).xlsx
+++ b/WT - Wheels, Wheel Bearing & Tires/Cost/WT A0100 (Wheel Assembly).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <definedName name="zer">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">BOM!$A$1:$N$18</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -586,12 +586,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
-    <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="\$#,##0.00_);&quot;($&quot;#,##0.00\)"/>
-    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="\$#,##0.00_);&quot;($&quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -1089,18 +1089,18 @@
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="2" borderId="3">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="6" fillId="2" borderId="3">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="108">
@@ -1111,7 +1111,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="11" fillId="0" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1121,11 +1121,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="172" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
@@ -1160,14 +1160,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="12" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1196,7 +1196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="37" fontId="4" fillId="0" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1209,13 +1209,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="173" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1231,18 +1231,18 @@
     <xf numFmtId="0" fontId="18" fillId="8" borderId="2" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="11" fillId="8" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="11" fillId="8" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="37" fontId="11" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="11" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="11" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="11" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1260,18 +1260,18 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="2" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="11" fillId="9" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="168" fontId="11" fillId="9" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="37" fontId="11" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="11" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="11" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="11" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1292,12 +1292,12 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="24" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="24" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="24" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="24" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="24" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="24" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="24" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1540,23 +1540,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1592,23 +1575,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2141,7 +2107,7 @@
   </sheetPr>
   <dimension ref="A1:O164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H10" sqref="H10"/>
       <selection pane="topRight" activeCell="H10" sqref="H10"/>
@@ -2359,7 +2325,7 @@
       <c r="F9" s="82"/>
       <c r="G9" s="83"/>
       <c r="H9" s="85">
-        <f t="shared" ref="H7:H17" si="0">SUM(J9:M9)</f>
+        <f t="shared" ref="H9:H17" si="0">SUM(J9:M9)</f>
         <v>0</v>
       </c>
       <c r="I9" s="91"/>
@@ -2368,7 +2334,7 @@
       <c r="L9" s="87"/>
       <c r="M9" s="87"/>
       <c r="N9" s="88">
-        <f t="shared" ref="N7:N17" si="1">H9*I9</f>
+        <f t="shared" ref="N9:N17" si="1">H9*I9</f>
         <v>0</v>
       </c>
       <c r="O9" s="89"/>
@@ -4876,8 +4842,8 @@
   </sheetPr>
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5145,7 +5111,7 @@
       </c>
       <c r="O10" s="49"/>
     </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="93">
         <v>10</v>
       </c>
@@ -5209,7 +5175,7 @@
       </c>
       <c r="O12" s="51"/>
     </row>
-    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="93">
         <v>30</v>
       </c>
@@ -5239,7 +5205,7 @@
       </c>
       <c r="O13" s="49"/>
     </row>
-    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="93">
         <v>40</v>
       </c>

</xml_diff>